<commit_message>
add automatically save report and update code for e2e and eApp Test flow
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Client/E2EFlow.xlsx
+++ b/src/test/resources/testdata/Client/E2EFlow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACD9B86-E165-4F46-8C9D-7C31C3402113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FACAC0-0AB3-49DA-87BB-4AE162ABA742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{176C0CDE-58DE-4F80-B9A9-A69CF69E117C}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="372">
   <si>
     <t>Alabama</t>
   </si>
@@ -1172,6 +1172,9 @@
   </si>
   <si>
     <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>Annuity_TaxQualification</t>
   </si>
 </sst>
 </file>
@@ -1598,7 +1601,7 @@
   <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1689,7 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>371</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
updated E2E flow excel and json file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Client/E2EFlow.xlsx
+++ b/src/test/resources/testdata/Client/E2EFlow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gxk0124\IdeaProjects\eApp-automation\src\test\resources\testdata\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F77B832-DCE7-45C0-BA30-733ABBDCEB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC33546E-9E3D-476E-A6E6-FDF805606DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{176C0CDE-58DE-4F80-B9A9-A69CF69E117C}"/>
   </bookViews>
@@ -1819,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40C238A-A12B-4AFE-B037-B65E78A076E7}">
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>